<commit_message>
fixed html to pdf and Pdf to excel
</commit_message>
<xml_diff>
--- a/convertExcel.xlsx
+++ b/convertExcel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="42">
   <si>
     <t xml:space="preserve">Segment</t>
   </si>
@@ -432,10 +432,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X32"/>
+  <dimension ref="A1:X63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U1" activeCellId="0" sqref="U:X"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L33" activeCellId="0" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2834,6 +2834,2021 @@
         <v>2014</v>
       </c>
     </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>1618.5</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G33" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H33" s="1" t="n">
+        <v>32370</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J33" s="1" t="n">
+        <v>32370</v>
+      </c>
+      <c r="K33" s="1" t="n">
+        <v>16185</v>
+      </c>
+      <c r="L33" s="1" t="n">
+        <v>16185</v>
+      </c>
+      <c r="M33" s="1" t="n">
+        <v>41640</v>
+      </c>
+      <c r="N33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P33" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q33" s="1" t="n">
+        <v>41640</v>
+      </c>
+      <c r="R33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T33" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U33" s="1" t="n">
+        <v>41640</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <v>1321</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G34" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H34" s="1" t="n">
+        <v>26420</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J34" s="1" t="n">
+        <v>26420</v>
+      </c>
+      <c r="K34" s="1" t="n">
+        <v>13210</v>
+      </c>
+      <c r="L34" s="1" t="n">
+        <v>13210</v>
+      </c>
+      <c r="M34" s="1" t="n">
+        <v>41640</v>
+      </c>
+      <c r="N34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P34" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q34" s="1" t="n">
+        <v>41640</v>
+      </c>
+      <c r="R34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T34" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U34" s="1" t="n">
+        <v>41640</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <v>2178</v>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G35" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="H35" s="1" t="n">
+        <v>32670</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J35" s="1" t="n">
+        <v>32670</v>
+      </c>
+      <c r="K35" s="1" t="n">
+        <v>21780</v>
+      </c>
+      <c r="L35" s="1" t="n">
+        <v>10890</v>
+      </c>
+      <c r="M35" s="1" t="n">
+        <v>41791</v>
+      </c>
+      <c r="N35" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="O35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P35" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q35" s="1" t="n">
+        <v>41791</v>
+      </c>
+      <c r="R35" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="S35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T35" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U35" s="1" t="n">
+        <v>41791</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" s="1" t="n">
+        <v>888</v>
+      </c>
+      <c r="F36" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G36" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="H36" s="1" t="n">
+        <v>13320</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J36" s="1" t="n">
+        <v>13320</v>
+      </c>
+      <c r="K36" s="1" t="n">
+        <v>8880</v>
+      </c>
+      <c r="L36" s="1" t="n">
+        <v>4440</v>
+      </c>
+      <c r="M36" s="1" t="n">
+        <v>41791</v>
+      </c>
+      <c r="N36" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="O36" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P36" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q36" s="1" t="n">
+        <v>41791</v>
+      </c>
+      <c r="R36" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="S36" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T36" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U36" s="1" t="n">
+        <v>41791</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="1" t="n">
+        <v>2470</v>
+      </c>
+      <c r="F37" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G37" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="H37" s="1" t="n">
+        <v>37050</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J37" s="1" t="n">
+        <v>37050</v>
+      </c>
+      <c r="K37" s="1" t="n">
+        <v>24700</v>
+      </c>
+      <c r="L37" s="1" t="n">
+        <v>12350</v>
+      </c>
+      <c r="M37" s="1" t="n">
+        <v>41791</v>
+      </c>
+      <c r="N37" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="O37" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P37" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q37" s="1" t="n">
+        <v>41791</v>
+      </c>
+      <c r="R37" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="S37" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T37" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U37" s="1" t="n">
+        <v>41791</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="1" t="n">
+        <v>1513</v>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G38" s="1" t="n">
+        <v>350</v>
+      </c>
+      <c r="H38" s="1" t="n">
+        <v>529550</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J38" s="1" t="n">
+        <v>529550</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L38" s="1" t="n">
+        <v>136170</v>
+      </c>
+      <c r="M38" s="1" t="n">
+        <v>41974</v>
+      </c>
+      <c r="N38" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O38" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P38" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q38" s="1" t="n">
+        <v>41974</v>
+      </c>
+      <c r="R38" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="S38" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T38" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U38" s="1" t="n">
+        <v>41974</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" s="1" t="n">
+        <v>921</v>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G39" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="H39" s="1" t="n">
+        <v>13815</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J39" s="1" t="n">
+        <v>13815</v>
+      </c>
+      <c r="K39" s="1" t="n">
+        <v>9210</v>
+      </c>
+      <c r="L39" s="1" t="n">
+        <v>4605</v>
+      </c>
+      <c r="M39" s="1" t="n">
+        <v>41699</v>
+      </c>
+      <c r="N39" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="O39" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P39" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q39" s="1" t="n">
+        <v>41699</v>
+      </c>
+      <c r="R39" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="S39" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="T39" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U39" s="1" t="n">
+        <v>41699</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="1" t="n">
+        <v>2518</v>
+      </c>
+      <c r="F40" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G40" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="H40" s="1" t="n">
+        <v>30216</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J40" s="1" t="n">
+        <v>30216</v>
+      </c>
+      <c r="K40" s="1" t="n">
+        <v>7554</v>
+      </c>
+      <c r="L40" s="1" t="n">
+        <v>22662</v>
+      </c>
+      <c r="M40" s="1" t="n">
+        <v>41791</v>
+      </c>
+      <c r="N40" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="O40" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P40" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q40" s="1" t="n">
+        <v>41791</v>
+      </c>
+      <c r="R40" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="S40" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T40" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U40" s="1" t="n">
+        <v>41791</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="1" t="n">
+        <v>1899</v>
+      </c>
+      <c r="F41" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G41" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H41" s="1" t="n">
+        <v>37980</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J41" s="1" t="n">
+        <v>37980</v>
+      </c>
+      <c r="K41" s="1" t="n">
+        <v>18990</v>
+      </c>
+      <c r="L41" s="1" t="n">
+        <v>18990</v>
+      </c>
+      <c r="M41" s="1" t="n">
+        <v>41791</v>
+      </c>
+      <c r="N41" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="O41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P41" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q41" s="1" t="n">
+        <v>41791</v>
+      </c>
+      <c r="R41" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="S41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T41" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U41" s="1" t="n">
+        <v>41791</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="1" t="n">
+        <v>1545</v>
+      </c>
+      <c r="F42" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G42" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="H42" s="1" t="n">
+        <v>18540</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J42" s="1" t="n">
+        <v>18540</v>
+      </c>
+      <c r="K42" s="1" t="n">
+        <v>4635</v>
+      </c>
+      <c r="L42" s="1" t="n">
+        <v>13905</v>
+      </c>
+      <c r="M42" s="1" t="n">
+        <v>41791</v>
+      </c>
+      <c r="N42" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="O42" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P42" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q42" s="1" t="n">
+        <v>41791</v>
+      </c>
+      <c r="R42" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="S42" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T42" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U42" s="1" t="n">
+        <v>41791</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" s="1" t="n">
+        <v>2470</v>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G43" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="H43" s="1" t="n">
+        <v>37050</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J43" s="1" t="n">
+        <v>37050</v>
+      </c>
+      <c r="K43" s="1" t="n">
+        <v>24700</v>
+      </c>
+      <c r="L43" s="1" t="n">
+        <v>12350</v>
+      </c>
+      <c r="M43" s="1" t="n">
+        <v>41791</v>
+      </c>
+      <c r="N43" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="O43" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P43" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q43" s="1" t="n">
+        <v>41791</v>
+      </c>
+      <c r="R43" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="S43" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T43" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U43" s="1" t="n">
+        <v>41791</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" s="1" t="n">
+        <v>2665.5</v>
+      </c>
+      <c r="F44" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G44" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="H44" s="1" t="n">
+        <v>333187.5</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J44" s="1" t="n">
+        <v>333187.5</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L44" s="1" t="n">
+        <v>13327.5</v>
+      </c>
+      <c r="M44" s="1" t="n">
+        <v>41821</v>
+      </c>
+      <c r="N44" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="O44" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P44" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q44" s="1" t="n">
+        <v>41821</v>
+      </c>
+      <c r="R44" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="S44" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="T44" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U44" s="1" t="n">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="1" t="n">
+        <v>958</v>
+      </c>
+      <c r="F45" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G45" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="H45" s="1" t="n">
+        <v>287400</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J45" s="1" t="n">
+        <v>287400</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L45" s="1" t="n">
+        <v>47900</v>
+      </c>
+      <c r="M45" s="1" t="n">
+        <v>41852</v>
+      </c>
+      <c r="N45" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="O45" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P45" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q45" s="1" t="n">
+        <v>41852</v>
+      </c>
+      <c r="R45" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="S45" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="T45" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U45" s="1" t="n">
+        <v>41852</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" s="1" t="n">
+        <v>2146</v>
+      </c>
+      <c r="F46" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G46" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="H46" s="1" t="n">
+        <v>15022</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J46" s="1" t="n">
+        <v>15022</v>
+      </c>
+      <c r="K46" s="1" t="n">
+        <v>10730</v>
+      </c>
+      <c r="L46" s="1" t="n">
+        <v>4292</v>
+      </c>
+      <c r="M46" s="1" t="n">
+        <v>41883</v>
+      </c>
+      <c r="N46" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="O46" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P46" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q46" s="1" t="n">
+        <v>41883</v>
+      </c>
+      <c r="R46" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="S46" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T46" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U46" s="1" t="n">
+        <v>41883</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E47" s="1" t="n">
+        <v>345</v>
+      </c>
+      <c r="F47" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G47" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="H47" s="1" t="n">
+        <v>43125</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J47" s="1" t="n">
+        <v>43125</v>
+      </c>
+      <c r="K47" s="1" t="n">
+        <v>41400</v>
+      </c>
+      <c r="L47" s="1" t="n">
+        <v>1725</v>
+      </c>
+      <c r="M47" s="1" t="n">
+        <v>41548</v>
+      </c>
+      <c r="N47" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="O47" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P47" s="1" t="n">
+        <v>2013</v>
+      </c>
+      <c r="Q47" s="1" t="n">
+        <v>41548</v>
+      </c>
+      <c r="R47" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="S47" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T47" s="1" t="n">
+        <v>2013</v>
+      </c>
+      <c r="U47" s="1" t="n">
+        <v>41548</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="1" t="n">
+        <v>615</v>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G48" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="H48" s="1" t="n">
+        <v>9225</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J48" s="1" t="n">
+        <v>9225</v>
+      </c>
+      <c r="K48" s="1" t="n">
+        <v>6150</v>
+      </c>
+      <c r="L48" s="1" t="n">
+        <v>3075</v>
+      </c>
+      <c r="M48" s="1" t="n">
+        <v>41974</v>
+      </c>
+      <c r="N48" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O48" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P48" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q48" s="1" t="n">
+        <v>41974</v>
+      </c>
+      <c r="R48" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="S48" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T48" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U48" s="1" t="n">
+        <v>41974</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49" s="1" t="n">
+        <v>292</v>
+      </c>
+      <c r="F49" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G49" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H49" s="1" t="n">
+        <v>5840</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J49" s="1" t="n">
+        <v>5840</v>
+      </c>
+      <c r="K49" s="1" t="n">
+        <v>2920</v>
+      </c>
+      <c r="L49" s="1" t="n">
+        <v>2920</v>
+      </c>
+      <c r="M49" s="1" t="n">
+        <v>41671</v>
+      </c>
+      <c r="N49" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="O49" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P49" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q49" s="1" t="n">
+        <v>41671</v>
+      </c>
+      <c r="R49" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S49" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T49" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U49" s="1" t="n">
+        <v>41671</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="1" t="n">
+        <v>974</v>
+      </c>
+      <c r="F50" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G50" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="H50" s="1" t="n">
+        <v>14610</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J50" s="1" t="n">
+        <v>14610</v>
+      </c>
+      <c r="K50" s="1" t="n">
+        <v>9740</v>
+      </c>
+      <c r="L50" s="1" t="n">
+        <v>4870</v>
+      </c>
+      <c r="M50" s="1" t="n">
+        <v>41671</v>
+      </c>
+      <c r="N50" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="O50" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P50" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q50" s="1" t="n">
+        <v>41671</v>
+      </c>
+      <c r="R50" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S50" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T50" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U50" s="1" t="n">
+        <v>41671</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="1" t="n">
+        <v>2518</v>
+      </c>
+      <c r="F51" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G51" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="H51" s="1" t="n">
+        <v>30216</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J51" s="1" t="n">
+        <v>30216</v>
+      </c>
+      <c r="K51" s="1" t="n">
+        <v>7554</v>
+      </c>
+      <c r="L51" s="1" t="n">
+        <v>22662</v>
+      </c>
+      <c r="M51" s="1" t="n">
+        <v>41791</v>
+      </c>
+      <c r="N51" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="O51" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P51" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q51" s="1" t="n">
+        <v>41791</v>
+      </c>
+      <c r="R51" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="S51" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T51" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U51" s="1" t="n">
+        <v>41791</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" s="1" t="n">
+        <v>1006</v>
+      </c>
+      <c r="F52" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G52" s="1" t="n">
+        <v>350</v>
+      </c>
+      <c r="H52" s="1" t="n">
+        <v>352100</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J52" s="1" t="n">
+        <v>352100</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L52" s="1" t="n">
+        <v>90540</v>
+      </c>
+      <c r="M52" s="1" t="n">
+        <v>41791</v>
+      </c>
+      <c r="N52" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="O52" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P52" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q52" s="1" t="n">
+        <v>41791</v>
+      </c>
+      <c r="R52" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="S52" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T52" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U52" s="1" t="n">
+        <v>41791</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" s="1" t="n">
+        <v>367</v>
+      </c>
+      <c r="F53" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G53" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="H53" s="1" t="n">
+        <v>4404</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J53" s="1" t="n">
+        <v>4404</v>
+      </c>
+      <c r="K53" s="1" t="n">
+        <v>1101</v>
+      </c>
+      <c r="L53" s="1" t="n">
+        <v>3303</v>
+      </c>
+      <c r="M53" s="1" t="n">
+        <v>41821</v>
+      </c>
+      <c r="N53" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="O53" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P53" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q53" s="1" t="n">
+        <v>41821</v>
+      </c>
+      <c r="R53" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="S53" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="T53" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U53" s="1" t="n">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="1" t="n">
+        <v>883</v>
+      </c>
+      <c r="F54" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G54" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="H54" s="1" t="n">
+        <v>6181</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J54" s="1" t="n">
+        <v>6181</v>
+      </c>
+      <c r="K54" s="1" t="n">
+        <v>4415</v>
+      </c>
+      <c r="L54" s="1" t="n">
+        <v>1766</v>
+      </c>
+      <c r="M54" s="1" t="n">
+        <v>41852</v>
+      </c>
+      <c r="N54" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="O54" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P54" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q54" s="1" t="n">
+        <v>41852</v>
+      </c>
+      <c r="R54" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="S54" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="T54" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U54" s="1" t="n">
+        <v>41852</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55" s="1" t="n">
+        <v>549</v>
+      </c>
+      <c r="F55" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G55" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="H55" s="1" t="n">
+        <v>8235</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J55" s="1" t="n">
+        <v>8235</v>
+      </c>
+      <c r="K55" s="1" t="n">
+        <v>5490</v>
+      </c>
+      <c r="L55" s="1" t="n">
+        <v>2745</v>
+      </c>
+      <c r="M55" s="1" t="n">
+        <v>41518</v>
+      </c>
+      <c r="N55" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="O55" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P55" s="1" t="n">
+        <v>2013</v>
+      </c>
+      <c r="Q55" s="1" t="n">
+        <v>41518</v>
+      </c>
+      <c r="R55" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="S55" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T55" s="1" t="n">
+        <v>2013</v>
+      </c>
+      <c r="U55" s="1" t="n">
+        <v>41518</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E56" s="1" t="n">
+        <v>788</v>
+      </c>
+      <c r="F56" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G56" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="H56" s="1" t="n">
+        <v>236400</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J56" s="1" t="n">
+        <v>236400</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L56" s="1" t="n">
+        <v>39400</v>
+      </c>
+      <c r="M56" s="1" t="n">
+        <v>41518</v>
+      </c>
+      <c r="N56" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="O56" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P56" s="1" t="n">
+        <v>2013</v>
+      </c>
+      <c r="Q56" s="1" t="n">
+        <v>41518</v>
+      </c>
+      <c r="R56" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="S56" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T56" s="1" t="n">
+        <v>2013</v>
+      </c>
+      <c r="U56" s="1" t="n">
+        <v>41518</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E57" s="1" t="n">
+        <v>2472</v>
+      </c>
+      <c r="F57" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G57" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="H57" s="1" t="n">
+        <v>37080</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J57" s="1" t="n">
+        <v>37080</v>
+      </c>
+      <c r="K57" s="1" t="n">
+        <v>24720</v>
+      </c>
+      <c r="L57" s="1" t="n">
+        <v>12360</v>
+      </c>
+      <c r="M57" s="1" t="n">
+        <v>41883</v>
+      </c>
+      <c r="N57" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="O57" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P57" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q57" s="1" t="n">
+        <v>41883</v>
+      </c>
+      <c r="R57" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="S57" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T57" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U57" s="1" t="n">
+        <v>41883</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E58" s="1" t="n">
+        <v>1143</v>
+      </c>
+      <c r="F58" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G58" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="H58" s="1" t="n">
+        <v>8001</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J58" s="1" t="n">
+        <v>8001</v>
+      </c>
+      <c r="K58" s="1" t="n">
+        <v>5715</v>
+      </c>
+      <c r="L58" s="1" t="n">
+        <v>2286</v>
+      </c>
+      <c r="M58" s="1" t="n">
+        <v>41913</v>
+      </c>
+      <c r="N58" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="O58" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P58" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q58" s="1" t="n">
+        <v>41913</v>
+      </c>
+      <c r="R58" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="S58" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T58" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U58" s="1" t="n">
+        <v>41913</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" s="1" t="n">
+        <v>1725</v>
+      </c>
+      <c r="F59" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G59" s="1" t="n">
+        <v>350</v>
+      </c>
+      <c r="H59" s="1" t="n">
+        <v>603750</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J59" s="1" t="n">
+        <v>603750</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L59" s="1" t="n">
+        <v>155250</v>
+      </c>
+      <c r="M59" s="1" t="n">
+        <v>41579</v>
+      </c>
+      <c r="N59" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="O59" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P59" s="1" t="n">
+        <v>2013</v>
+      </c>
+      <c r="Q59" s="1" t="n">
+        <v>41579</v>
+      </c>
+      <c r="R59" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="S59" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T59" s="1" t="n">
+        <v>2013</v>
+      </c>
+      <c r="U59" s="1" t="n">
+        <v>41579</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60" s="1" t="n">
+        <v>912</v>
+      </c>
+      <c r="F60" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G60" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="H60" s="1" t="n">
+        <v>10944</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J60" s="1" t="n">
+        <v>10944</v>
+      </c>
+      <c r="K60" s="1" t="n">
+        <v>2736</v>
+      </c>
+      <c r="L60" s="1" t="n">
+        <v>8208</v>
+      </c>
+      <c r="M60" s="1" t="n">
+        <v>41579</v>
+      </c>
+      <c r="N60" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="O60" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P60" s="1" t="n">
+        <v>2013</v>
+      </c>
+      <c r="Q60" s="1" t="n">
+        <v>41579</v>
+      </c>
+      <c r="R60" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="S60" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T60" s="1" t="n">
+        <v>2013</v>
+      </c>
+      <c r="U60" s="1" t="n">
+        <v>41579</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E61" s="1" t="n">
+        <v>2152</v>
+      </c>
+      <c r="F61" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G61" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="H61" s="1" t="n">
+        <v>32280</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J61" s="1" t="n">
+        <v>32280</v>
+      </c>
+      <c r="K61" s="1" t="n">
+        <v>21520</v>
+      </c>
+      <c r="L61" s="1" t="n">
+        <v>10760</v>
+      </c>
+      <c r="M61" s="1" t="n">
+        <v>41609</v>
+      </c>
+      <c r="N61" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O61" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P61" s="1" t="n">
+        <v>2013</v>
+      </c>
+      <c r="Q61" s="1" t="n">
+        <v>41609</v>
+      </c>
+      <c r="R61" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="S61" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T61" s="1" t="n">
+        <v>2013</v>
+      </c>
+      <c r="U61" s="1" t="n">
+        <v>41609</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E62" s="1" t="n">
+        <v>1817</v>
+      </c>
+      <c r="F62" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G62" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H62" s="1" t="n">
+        <v>36340</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J62" s="1" t="n">
+        <v>36340</v>
+      </c>
+      <c r="K62" s="1" t="n">
+        <v>18170</v>
+      </c>
+      <c r="L62" s="1" t="n">
+        <v>18170</v>
+      </c>
+      <c r="M62" s="1" t="n">
+        <v>41974</v>
+      </c>
+      <c r="N62" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O62" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P62" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q62" s="1" t="n">
+        <v>41974</v>
+      </c>
+      <c r="R62" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="S62" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T62" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U62" s="1" t="n">
+        <v>41974</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E63" s="1" t="n">
+        <v>1513</v>
+      </c>
+      <c r="F63" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G63" s="1" t="n">
+        <v>350</v>
+      </c>
+      <c r="H63" s="1" t="n">
+        <v>529550</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J63" s="1" t="n">
+        <v>529550</v>
+      </c>
+      <c r="K63" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L63" s="1" t="n">
+        <v>136170</v>
+      </c>
+      <c r="M63" s="1" t="n">
+        <v>41974</v>
+      </c>
+      <c r="N63" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O63" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P63" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="Q63" s="1" t="n">
+        <v>41974</v>
+      </c>
+      <c r="R63" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="S63" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T63" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="U63" s="1" t="n">
+        <v>41974</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>